<commit_message>
Do a bit more VDU stuff.
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/beeb/mos320/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BF4BE7-6D24-3540-B139-F8FE1C1BB45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7575467-8E4A-634F-A1A3-0F238D132BCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="460" windowWidth="28800" windowHeight="20540" xr2:uid="{683AEA06-EB3E-E344-82FE-582ED2CFF1BD}"/>
+    <workbookView xWindow="28800" yWindow="4300" windowWidth="28800" windowHeight="20540" xr2:uid="{683AEA06-EB3E-E344-82FE-582ED2CFF1BD}"/>
   </bookViews>
   <sheets>
     <sheet name="OSBYTEs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>OSBYTE (dec)</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>MasRef page</t>
+  </si>
+  <si>
+    <t>paged mode counter</t>
   </si>
 </sst>
 </file>
@@ -433,7 +436,7 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -665,6 +668,9 @@
         <f t="shared" si="3"/>
         <v>269</v>
       </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">

</xml_diff>